<commit_message>
Gradient descent solution added 2
</commit_message>
<xml_diff>
--- a/ML - Gradient Descent/Source/Vibrations.xlsx
+++ b/ML - Gradient Descent/Source/Vibrations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1e08ceff118239cf/Desktop/Programming/Python/ML - Gradient Descent/Source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABD40943-F216-4A9F-B06B-B590A79B51BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{ABD40943-F216-4A9F-B06B-B590A79B51BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A17FAC26-424C-4CF2-AE7D-A8E18DDC7081}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD60C24C-57D7-4EC9-9546-F4BD3712AA4B}"/>
   </bookViews>
@@ -900,6 +900,20 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'[1]Sound-and-vibrations'!$A$2:$A$21</c:f>
@@ -3000,8 +3014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62CD9D7B-DC4E-4FCD-9C02-9E01C111DDA5}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>